<commit_message>
estilização das abas copiadas
</commit_message>
<xml_diff>
--- a/outputs/expansao_atualizado_form4.xlsx
+++ b/outputs/expansao_atualizado_form4.xlsx
@@ -726,7 +726,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="8" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFAD0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3868,41 +3948,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6110,41 +6190,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8352,41 +8432,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10594,41 +10674,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12836,41 +12916,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15078,41 +15158,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33193,6 +33273,246 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D3:P9 E2:P2">
+    <cfRule type="cellIs" priority="319" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="320" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="321" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="322" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="323" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="324" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M9">
+    <cfRule type="cellIs" priority="277" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="278" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="279" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="280" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="281" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="282" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N9">
+    <cfRule type="cellIs" priority="271" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="272" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="273" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="274" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="275" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="276" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O9">
+    <cfRule type="cellIs" priority="265" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="266" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="267" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="268" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="269" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="270" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P9">
+    <cfRule type="cellIs" priority="259" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="260" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="261" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="262" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="263" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="264" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:P9">
+    <cfRule type="cellIs" priority="37" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="38" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="39" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="40" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="41" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="42" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:P24">
+    <cfRule type="cellIs" priority="31" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="32" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="33" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="34" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="35" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="36" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:P35">
+    <cfRule type="cellIs" priority="25" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="26" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="27" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="28" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="29" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="30" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:P40">
+    <cfRule type="cellIs" priority="19" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="20" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="21" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="22" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="23" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="24" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:P50">
+    <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="14" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="15" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="16" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="17" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:P60">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:P70">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -51156,6 +51476,192 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D3:P9 E2:P2">
+    <cfRule type="cellIs" priority="79" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="80" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="81" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="82" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="83" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="84" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="49" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="50" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="51" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="52" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="53" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="54" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M9">
+    <cfRule type="cellIs" priority="73" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="74" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="75" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="76" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="77" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="78" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N9">
+    <cfRule type="cellIs" priority="67" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="68" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="69" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="70" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="71" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="72" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O9">
+    <cfRule type="cellIs" priority="61" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="62" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="63" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="64" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="65" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="66" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P9">
+    <cfRule type="cellIs" priority="55" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="56" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="57" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="58" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="59" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="60" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:P70">
+    <cfRule type="cellIs" priority="13" operator="equal" dxfId="0">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="14" operator="equal" dxfId="1">
+      <formula>"UVR Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="15" operator="equal" dxfId="2">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="16" operator="equal" dxfId="3">
+      <formula>"Atrasado &gt;= 2"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="17" operator="equal" dxfId="4">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="equal" dxfId="5">
+      <formula>"Enviado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:P9">
+    <cfRule type="cellIs" priority="12" operator="equal" dxfId="6">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:P24">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="7">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:P35">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="6">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="7">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:P40">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="6">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="7">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:P50">
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="6">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="7">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:P60">
+    <cfRule type="cellIs" priority="2" operator="equal" dxfId="6">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="7">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -53841,41 +54347,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56583,41 +57089,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59345,41 +59851,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62103,41 +62609,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -64789,41 +65295,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67039,41 +67545,41 @@
   </sheetData>
   <autoFilter ref="A1:G1"/>
   <conditionalFormatting sqref="G2:G58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J58">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="8" stopIfTrue="1">
       <formula>"Sim"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="9" stopIfTrue="1">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="10" stopIfTrue="1">
       <formula>"Em Análise"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="11" stopIfTrue="1">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="12" stopIfTrue="1">
       <formula>"Atrasado"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="13" stopIfTrue="1">
       <formula>"Atrasado &gt;= 2"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Outras Ocorrências"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="7" stopIfTrue="1">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="15" stopIfTrue="1">
       <formula>"Sem Técnico"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" dxfId="6" stopIfTrue="1">
+    <cfRule type="cellIs" priority="11" operator="equal" dxfId="14" stopIfTrue="1">
       <formula>"Duplicado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>